<commit_message>
Freeze row 1 of anotherExample.xlsx
</commit_message>
<xml_diff>
--- a/workingWithExcelSpreadsheets/anotherExample.xlsx
+++ b/workingWithExcelSpreadsheets/anotherExample.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,14 @@
       <b val="1"/>
       <color rgb="00FF0000"/>
       <sz val="24"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,9 +60,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -352,31 +362,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15"/>
+    <col customWidth="1" max="2" min="2" width="20"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>PRODUCE</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>COST PER POUND</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>POUNDS SOLD</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
@@ -462,7 +479,33 @@
         <v>18.02</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>This cell is going to be merged up to D7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pear</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add a chart to anotherExample.xlsx file from terminal
</commit_message>
<xml_diff>
--- a/workingWithExcelSpreadsheets/anotherExample.xlsx
+++ b/workingWithExcelSpreadsheets/anotherExample.xlsx
@@ -71,6 +71,108 @@
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>My test chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Produce Sales</v>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'sheet1'!$A$1:$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,10 +502,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Garlic</t>
-        </is>
+      <c r="A2" t="n">
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>1.19</v>
@@ -416,10 +516,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Potatoes</t>
-        </is>
+      <c r="A3" t="n">
+        <v>3</v>
       </c>
       <c r="B3" t="n">
         <v>0.86</v>
@@ -432,10 +530,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Okra</t>
-        </is>
+      <c r="A4" t="n">
+        <v>4</v>
       </c>
       <c r="B4" t="n">
         <v>2.26</v>
@@ -448,10 +544,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Fava beans</t>
-        </is>
+      <c r="A5" t="n">
+        <v>5</v>
       </c>
       <c r="B5" t="n">
         <v>2.69</v>
@@ -464,10 +558,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Watermelon</t>
-        </is>
+      <c r="A6" t="n">
+        <v>6</v>
       </c>
       <c r="B6" t="n">
         <v>0.66</v>
@@ -480,17 +572,13 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>This cell is going to be merged up to D7</t>
-        </is>
+      <c r="A7" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Pear</t>
-        </is>
+      <c r="A8" t="n">
+        <v>8</v>
       </c>
       <c r="B8" t="n">
         <v>1.09</v>
@@ -507,6 +595,7 @@
     <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>